<commit_message>
3.3.1 files from RMI
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
+++ b/InputData/add-outputs/SCoC/Social Cost of Carbon.xlsx
@@ -1,27 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\add-outputs\SCoC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\All_states_RMI\MN\add-outputs\SCoC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A1A1536-0B48-4C82-B1F6-B7DD8F9747F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="21075" windowHeight="11820"/>
+    <workbookView xWindow="1150" yWindow="570" windowWidth="16460" windowHeight="13230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="SourceData" sheetId="2" r:id="rId2"/>
     <sheet name="SCoC" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Source:</t>
   </si>
@@ -88,11 +100,14 @@
   <si>
     <t>ton of carbon dioxide emitted, the U.S. government typically uses the figures based on</t>
   </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
@@ -236,7 +251,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -257,16 +272,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Body: normal cell" xfId="5"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="3"/>
-    <cellStyle name="Footnotes: top row" xfId="7"/>
-    <cellStyle name="Header: bottom row" xfId="4"/>
+    <cellStyle name="Body: normal cell" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Parent row" xfId="6"/>
-    <cellStyle name="Table title" xfId="2"/>
+    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Table title" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -357,6 +373,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -392,6 +425,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -567,24 +617,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="97.140625" customWidth="1"/>
+    <col min="2" max="2" width="97.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="14">
+        <v>44509</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,67 +648,67 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="13">
         <v>1.109</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>15</v>
       </c>
@@ -664,18 +720,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="7" max="7" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
@@ -691,7 +747,7 @@
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -723,7 +779,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -755,7 +811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="13">
         <v>2010</v>
       </c>
@@ -792,7 +848,7 @@
         <v>9.5373999999999999E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="13">
         <v>2011</v>
       </c>
@@ -829,7 +885,7 @@
         <v>9.9810000000000008E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="13">
         <v>2012</v>
       </c>
@@ -866,7 +922,7 @@
         <v>1.03137E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="13">
         <v>2013</v>
       </c>
@@ -903,7 +959,7 @@
         <v>1.0757299999999999E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="13">
         <v>2014</v>
       </c>
@@ -940,7 +996,7 @@
         <v>1.12009E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="13">
         <v>2015</v>
       </c>
@@ -977,7 +1033,7 @@
         <v>1.1644499999999999E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="13">
         <v>2016</v>
       </c>
@@ -1014,7 +1070,7 @@
         <v>1.1977199999999999E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="13">
         <v>2017</v>
       </c>
@@ -1051,7 +1107,7 @@
         <v>1.24208E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="13">
         <v>2018</v>
       </c>
@@ -1088,7 +1144,7 @@
         <v>1.28644E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="13">
         <v>2019</v>
       </c>
@@ -1125,7 +1181,7 @@
         <v>1.3307999999999999E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="13">
         <v>2020</v>
       </c>
@@ -1162,7 +1218,7 @@
         <v>1.3640700000000001E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="13">
         <v>2021</v>
       </c>
@@ -1199,7 +1255,7 @@
         <v>1.39734E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="13">
         <v>2022</v>
       </c>
@@ -1236,7 +1292,7 @@
         <v>1.4306100000000002E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="13">
         <v>2023</v>
       </c>
@@ -1273,7 +1329,7 @@
         <v>1.4638800000000001E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="13">
         <v>2024</v>
       </c>
@@ -1310,7 +1366,7 @@
         <v>1.49715E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="13">
         <v>2025</v>
       </c>
@@ -1347,7 +1403,7 @@
         <v>1.5304199999999999E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="13">
         <v>2026</v>
       </c>
@@ -1384,7 +1440,7 @@
         <v>1.5636900000000001E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="13">
         <v>2027</v>
       </c>
@@ -1421,7 +1477,7 @@
         <v>1.5858699999999999E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="13">
         <v>2028</v>
       </c>
@@ -1458,7 +1514,7 @@
         <v>1.6191399999999998E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="13">
         <v>2029</v>
       </c>
@@ -1495,7 +1551,7 @@
         <v>1.65241E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="13">
         <v>2030</v>
       </c>
@@ -1532,7 +1588,7 @@
         <v>1.6856799999999999E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="13">
         <v>2031</v>
       </c>
@@ -1569,7 +1625,7 @@
         <v>1.7189500000000001E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="13">
         <v>2032</v>
       </c>
@@ -1606,7 +1662,7 @@
         <v>1.75222E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="13">
         <v>2033</v>
       </c>
@@ -1643,7 +1699,7 @@
         <v>1.7854900000000001E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="13">
         <v>2034</v>
       </c>
@@ -1680,7 +1736,7 @@
         <v>1.81876E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="13">
         <v>2035</v>
       </c>
@@ -1717,7 +1773,7 @@
         <v>1.86312E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="13">
         <v>2036</v>
       </c>
@@ -1754,7 +1810,7 @@
         <v>1.8963900000000002E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="13">
         <v>2037</v>
       </c>
@@ -1791,7 +1847,7 @@
         <v>1.9296600000000001E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="13">
         <v>2038</v>
       </c>
@@ -1828,7 +1884,7 @@
         <v>1.96293E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="13">
         <v>2039</v>
       </c>
@@ -1865,7 +1921,7 @@
         <v>1.9962000000000002E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="13">
         <v>2040</v>
       </c>
@@ -1902,7 +1958,7 @@
         <v>2.0294700000000001E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="13">
         <v>2041</v>
       </c>
@@ -1939,7 +1995,7 @@
         <v>2.06274E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="13">
         <v>2042</v>
       </c>
@@ -1976,7 +2032,7 @@
         <v>2.0960099999999999E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="13">
         <v>2043</v>
       </c>
@@ -2013,7 +2069,7 @@
         <v>2.1292800000000001E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="13">
         <v>2044</v>
       </c>
@@ -2050,7 +2106,7 @@
         <v>2.1514599999999999E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="13">
         <v>2045</v>
       </c>
@@ -2087,7 +2143,7 @@
         <v>2.1847299999999998E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="13">
         <v>2046</v>
       </c>
@@ -2124,7 +2180,7 @@
         <v>2.2180000000000002E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="13">
         <v>2047</v>
       </c>
@@ -2161,7 +2217,7 @@
         <v>2.2512700000000001E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="13">
         <v>2048</v>
       </c>
@@ -2198,7 +2254,7 @@
         <v>2.2845400000000001E-4</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="13">
         <v>2049</v>
       </c>
@@ -2235,7 +2291,7 @@
         <v>2.31781E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="13">
         <v>2050</v>
       </c>
@@ -2278,7 +2334,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -2288,12 +2344,12 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -2301,7 +2357,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <f>SourceData!G4</f>
         <v>2010</v>
@@ -2311,7 +2367,7 @@
         <v>3.4378999999999997E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>SourceData!G5</f>
         <v>2011</v>
@@ -2321,7 +2377,7 @@
         <v>3.5487999999999996E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <f>SourceData!G6</f>
         <v>2012</v>
@@ -2331,7 +2387,7 @@
         <v>3.6597000000000002E-5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <f>SourceData!G7</f>
         <v>2013</v>
@@ -2341,7 +2397,7 @@
         <v>3.7706000000000001E-5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <f>SourceData!G8</f>
         <v>2014</v>
@@ -2351,7 +2407,7 @@
         <v>3.8815E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <f>SourceData!G9</f>
         <v>2015</v>
@@ -2361,7 +2417,7 @@
         <v>3.9923999999999999E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <f>SourceData!G10</f>
         <v>2016</v>
@@ -2371,7 +2427,7 @@
         <v>4.2141999999999997E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <f>SourceData!G11</f>
         <v>2017</v>
@@ -2381,7 +2437,7 @@
         <v>4.3250999999999996E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <f>SourceData!G12</f>
         <v>2018</v>
@@ -2391,7 +2447,7 @@
         <v>4.4360000000000002E-5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <f>SourceData!G13</f>
         <v>2019</v>
@@ -2401,7 +2457,7 @@
         <v>4.5469000000000001E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <f>SourceData!G14</f>
         <v>2020</v>
@@ -2411,7 +2467,7 @@
         <v>4.6578E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <f>SourceData!G15</f>
         <v>2021</v>
@@ -2421,7 +2477,7 @@
         <v>4.6578E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <f>SourceData!G16</f>
         <v>2022</v>
@@ -2431,7 +2487,7 @@
         <v>4.7686999999999999E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <f>SourceData!G17</f>
         <v>2023</v>
@@ -2441,7 +2497,7 @@
         <v>4.8795999999999998E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <f>SourceData!G18</f>
         <v>2024</v>
@@ -2451,7 +2507,7 @@
         <v>4.9905000000000004E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <f>SourceData!G19</f>
         <v>2025</v>
@@ -2461,7 +2517,7 @@
         <v>5.1013999999999996E-5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <f>SourceData!G20</f>
         <v>2026</v>
@@ -2471,7 +2527,7 @@
         <v>5.2122999999999995E-5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <f>SourceData!G21</f>
         <v>2027</v>
@@ -2481,7 +2537,7 @@
         <v>5.3232000000000001E-5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <f>SourceData!G22</f>
         <v>2028</v>
@@ -2491,7 +2547,7 @@
         <v>5.4341E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <f>SourceData!G23</f>
         <v>2029</v>
@@ -2501,7 +2557,7 @@
         <v>5.4341E-5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <f>SourceData!G24</f>
         <v>2030</v>
@@ -2511,7 +2567,7 @@
         <v>5.5450000000000006E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <f>SourceData!G25</f>
         <v>2031</v>
@@ -2521,7 +2577,7 @@
         <v>5.6558999999999998E-5</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <f>SourceData!G26</f>
         <v>2032</v>
@@ -2531,7 +2587,7 @@
         <v>5.7667999999999997E-5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <f>SourceData!G27</f>
         <v>2033</v>
@@ -2541,7 +2597,7 @@
         <v>5.8777000000000003E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <f>SourceData!G28</f>
         <v>2034</v>
@@ -2551,7 +2607,7 @@
         <v>5.9885999999999995E-5</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <f>SourceData!G29</f>
         <v>2035</v>
@@ -2561,7 +2617,7 @@
         <v>6.0994999999999995E-5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <f>SourceData!G30</f>
         <v>2036</v>
@@ -2571,7 +2627,7 @@
         <v>6.2104E-5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <f>SourceData!G31</f>
         <v>2037</v>
@@ -2581,7 +2637,7 @@
         <v>6.3213000000000006E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
         <f>SourceData!G32</f>
         <v>2038</v>
@@ -2591,7 +2647,7 @@
         <v>6.4321999999999998E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31">
         <f>SourceData!G33</f>
         <v>2039</v>
@@ -2601,7 +2657,7 @@
         <v>6.5430999999999991E-5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32">
         <f>SourceData!G34</f>
         <v>2040</v>
@@ -2611,7 +2667,7 @@
         <v>6.6539999999999997E-5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <f>SourceData!G35</f>
         <v>2041</v>
@@ -2621,7 +2677,7 @@
         <v>6.7649000000000002E-5</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <f>SourceData!G36</f>
         <v>2042</v>
@@ -2631,7 +2687,7 @@
         <v>6.7649000000000002E-5</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <f>SourceData!G37</f>
         <v>2043</v>
@@ -2641,7 +2697,7 @@
         <v>6.8757999999999995E-5</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <f>SourceData!G38</f>
         <v>2044</v>
@@ -2651,7 +2707,7 @@
         <v>6.9867E-5</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <f>SourceData!G39</f>
         <v>2045</v>
@@ -2661,7 +2717,7 @@
         <v>7.0975999999999993E-5</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38">
         <f>SourceData!G40</f>
         <v>2046</v>
@@ -2671,7 +2727,7 @@
         <v>7.2084999999999998E-5</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
         <f>SourceData!G41</f>
         <v>2047</v>
@@ -2681,7 +2737,7 @@
         <v>7.3194000000000004E-5</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
         <f>SourceData!G42</f>
         <v>2048</v>
@@ -2691,7 +2747,7 @@
         <v>7.4302999999999997E-5</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41">
         <f>SourceData!G43</f>
         <v>2049</v>
@@ -2701,7 +2757,7 @@
         <v>7.5412000000000002E-5</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42">
         <f>SourceData!G44</f>
         <v>2050</v>

</xml_diff>